<commit_message>
api,adeguamenti excel + strcture fe
</commit_message>
<xml_diff>
--- a/db/film.xlsx
+++ b/db/film.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuse\Desktop\projects\cineMille\cineMille\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D9DFF18-DC8E-422F-86E5-024F6303DC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A129586-3325-433F-A400-609281A78ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="2850" windowWidth="15375" windowHeight="7875" xr2:uid="{7C168252-3A4F-4C95-9485-B9052648DEE4}"/>
+    <workbookView xWindow="3705" yWindow="2970" windowWidth="15375" windowHeight="7875" xr2:uid="{7C168252-3A4F-4C95-9485-B9052648DEE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Fury</t>
+  </si>
+  <si>
+    <t>durata</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC7B7B8-F983-4F42-B7CE-F72BB5C2E40E}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +421,7 @@
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +434,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -442,8 +448,11 @@
       <c r="C2" s="1">
         <v>43739</v>
       </c>
+      <c r="E2">
+        <v>120</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -453,8 +462,11 @@
       <c r="C3" s="1">
         <v>40445</v>
       </c>
+      <c r="E3">
+        <v>150</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -463,6 +475,9 @@
       </c>
       <c r="C4" s="1">
         <v>42157</v>
+      </c>
+      <c r="E4">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>